<commit_message>
Replace CO2_per_mode.xlsx with new version! Including diet and type of car!
</commit_message>
<xml_diff>
--- a/CO2_per_mode.xlsx
+++ b/CO2_per_mode.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Joachim/Documents/ETH/Courses/Smart Energy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Joachim/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C0E508-B95F-2E45-A4B7-477318505CD4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401EB1C4-A762-334C-8A7B-F3B665622486}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21620" windowHeight="15540" xr2:uid="{0B26FDAA-DC1F-A14B-ACA1-10A61190EA9B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{0B26FDAA-DC1F-A14B-ACA1-10A61190EA9B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Overview" sheetId="2" r:id="rId1"/>
+    <sheet name="Calculations &amp; sources" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="47">
   <si>
     <t>Air</t>
   </si>
@@ -74,9 +75,6 @@
     <t xml:space="preserve">g(CO2)/km </t>
   </si>
   <si>
-    <t xml:space="preserve">40-100 </t>
-  </si>
-  <si>
     <t xml:space="preserve">Average: </t>
   </si>
   <si>
@@ -105,13 +103,96 @@
   </si>
   <si>
     <t>https://www.bbc.com/news/science-environment-49349566</t>
+  </si>
+  <si>
+    <t>Source:</t>
+  </si>
+  <si>
+    <t>http://web.mit.edu/2.813/www/readings/DrivingVsWalking.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source: SBB </t>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="26"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>SBB Ecocalculator </t>
+    </r>
+  </si>
+  <si>
+    <t>Background Report </t>
+  </si>
+  <si>
+    <t>Version 1.1, October 2011 </t>
+  </si>
+  <si>
+    <t>Car Lux</t>
+  </si>
+  <si>
+    <t>Car Med</t>
+  </si>
+  <si>
+    <t>Car Small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not used in app </t>
+  </si>
+  <si>
+    <t>REFRERENCE! Not very general! Switzerlannd specific! Trying to make it more or less EUROPE specific!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normal diet </t>
+  </si>
+  <si>
+    <t xml:space="preserve">plant based </t>
+  </si>
+  <si>
+    <t>meat based</t>
+  </si>
+  <si>
+    <t>Not considering diet!</t>
+  </si>
+  <si>
+    <t>Bus innercity!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bus (Coach) </t>
+  </si>
+  <si>
+    <t>ca. 50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carbon Emissions in g/Person*km </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 mile = </t>
+  </si>
+  <si>
+    <t>vegan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">typical </t>
+  </si>
+  <si>
+    <t>walking</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.00000"/>
+  </numFmts>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -144,6 +225,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -259,7 +382,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -276,6 +399,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -298,6 +430,122 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>939800</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="https://lh6.googleusercontent.com/53Hdi36DScpLEKRm8dooUr-mPcM7MFCfuK218tqc4iptPRwSuhRajHWHKkA-xMDSaClSCGuxnuTNFeelg-gtOEgh9CEoyoX6NNQmOYB8r2Sg46LMvBO2gzogkNbydulu7W6Uei1a">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CB03D09-6F0B-E844-9E37-03A596E60CC1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="825500" y="4114800"/>
+          <a:ext cx="7645400" cy="2222500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97A7DEF5-DE0D-3648-B3DF-4522B58C3EC3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="825500" y="7366000"/>
+          <a:ext cx="4775200" cy="6261100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -596,11 +844,148 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50943F23-9A78-2A4D-85EB-B0F06C32EBC1}">
+  <dimension ref="C5:O11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="5" spans="3:15" ht="24" x14ac:dyDescent="0.3">
+      <c r="C5" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="21"/>
+      <c r="M6" s="21"/>
+    </row>
+    <row r="7" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="O7" s="11"/>
+    </row>
+    <row r="8" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8">
+        <f>E1</f>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f>(F1+24.9)/2</f>
+        <v>12.45</v>
+      </c>
+      <c r="G8" t="e">
+        <f>((#REF!+100.3)/2)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8">
+        <f>(256.2+203.8+254.6)/3</f>
+        <v>238.20000000000002</v>
+      </c>
+      <c r="J8">
+        <f>(201.3+159.5+200)/3</f>
+        <v>186.93333333333331</v>
+      </c>
+      <c r="K8">
+        <f>(122+103.9+134.7)/3</f>
+        <v>120.2</v>
+      </c>
+      <c r="L8" s="4">
+        <v>72</v>
+      </c>
+      <c r="O8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="M9">
+        <v>10.770460768596649</v>
+      </c>
+      <c r="N9">
+        <v>19.883927572793816</v>
+      </c>
+      <c r="O9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="M10">
+        <v>53.852303842983247</v>
+      </c>
+      <c r="N10">
+        <v>95.277152952970354</v>
+      </c>
+      <c r="O10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="M11">
+        <v>124.27454732996134</v>
+      </c>
+      <c r="N11">
+        <v>186.41182099494202</v>
+      </c>
+      <c r="O11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E23E3A-C6DA-394A-B55A-2BD6A19E6576}">
-  <dimension ref="A2:M17"/>
+  <dimension ref="A2:N90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15:I15"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -687,7 +1072,7 @@
         <v>68</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H6" s="6">
         <f>(104+158)/2</f>
@@ -703,7 +1088,7 @@
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -717,7 +1102,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H7" s="6">
         <v>128</v>
@@ -736,16 +1121,14 @@
       <c r="C8" s="6">
         <v>250</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6">
         <f>(30+60)/2</f>
         <v>45</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H8" s="6">
         <v>200</v>
@@ -757,7 +1140,7 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -771,7 +1154,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H9" s="6">
         <v>101</v>
@@ -781,7 +1164,7 @@
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
       <c r="M9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -795,7 +1178,7 @@
         <v>18.8</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -803,7 +1186,7 @@
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
       <c r="M10" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -829,7 +1212,7 @@
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="M11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -865,8 +1248,8 @@
         <v>238.5</v>
       </c>
       <c r="D14" s="8">
-        <f>AVERAGE(D6:D9)</f>
-        <v>34</v>
+        <f>AVERAGE(D6:D11)</f>
+        <v>31.375</v>
       </c>
       <c r="E14" s="8">
         <f>AVERAGE(E5:E13)</f>
@@ -894,7 +1277,7 @@
     </row>
     <row r="15" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="3">
@@ -903,7 +1286,7 @@
       </c>
       <c r="D15" s="4">
         <f>D14</f>
-        <v>34</v>
+        <v>31.375</v>
       </c>
       <c r="E15" s="4">
         <f>E14</f>
@@ -914,11 +1297,11 @@
         <v>43.933333333333337</v>
       </c>
       <c r="G15" s="4"/>
-      <c r="H15" s="16">
+      <c r="H15" s="25">
         <f>AVERAGE(H14:I14)</f>
         <v>98.616666666666674</v>
       </c>
-      <c r="I15" s="17"/>
+      <c r="I15" s="26"/>
       <c r="J15" s="4">
         <f>J14</f>
         <v>72</v>
@@ -932,24 +1315,599 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K16" t="s">
+        <v>15</v>
+      </c>
+      <c r="L16" t="s">
         <v>16</v>
       </c>
-      <c r="L16" t="s">
+    </row>
+    <row r="17" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="K17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K17" t="s">
+    <row r="21" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="H21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="H23" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
+        <v>43</v>
+      </c>
+      <c r="I26" s="23">
+        <v>1.60934</v>
+      </c>
+    </row>
+    <row r="28" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="I28" t="s">
+        <v>10</v>
+      </c>
+      <c r="J28" t="s">
+        <v>44</v>
+      </c>
+      <c r="K28">
+        <f>26/(I26*1.5)</f>
+        <v>10.770460768596649</v>
+      </c>
+      <c r="M28">
+        <f>1000/(1.6*1.5)</f>
+        <v>416.66666666666663</v>
+      </c>
+    </row>
+    <row r="29" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="J29" t="s">
+        <v>45</v>
+      </c>
+      <c r="K29">
+        <f>130/(I26*1.5)</f>
+        <v>53.852303842983247</v>
+      </c>
+    </row>
+    <row r="30" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="J30" t="s">
+        <v>37</v>
+      </c>
+      <c r="K30">
+        <f>300/(I26*1.5)</f>
+        <v>124.27454732996134</v>
+      </c>
+    </row>
+    <row r="32" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="I32" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="J32" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="K32" s="24">
+        <f>48/(I26*1.5)</f>
+        <v>19.883927572793816</v>
+      </c>
+    </row>
+    <row r="33" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="I33" s="24"/>
+      <c r="J33" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="K33" s="24">
+        <f>230/(I26*1.5)</f>
+        <v>95.277152952970354</v>
+      </c>
+    </row>
+    <row r="34" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="I34" s="24"/>
+      <c r="J34" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="K34" s="24">
+        <f>450/(I26*1.5)</f>
+        <v>186.41182099494202</v>
+      </c>
+    </row>
+    <row r="36" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="7:11" ht="33" x14ac:dyDescent="0.35">
+      <c r="G37" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="7:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="G38" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G39" s="18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G46" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="56" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F56">
+        <f>(201.3+159.5+200)/3</f>
+        <v>186.93333333333331</v>
+      </c>
+    </row>
+    <row r="59" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F59">
+        <f>(122+103.9+134.7)/3</f>
+        <v>120.2</v>
+      </c>
+    </row>
+    <row r="63" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F63">
+        <f>(256.2+203.8+254.6)/3</f>
+        <v>238.20000000000002</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C69" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E69" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F69" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G69" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H69" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I69" s="12"/>
+      <c r="J69" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="K69" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L69" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B70" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G70" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H70" s="9"/>
+      <c r="I70" s="9"/>
+      <c r="J70" s="9"/>
+      <c r="K70" s="9"/>
+      <c r="L70" s="9"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B71" s="6"/>
+      <c r="C71" s="6">
+        <v>285</v>
+      </c>
+      <c r="D71" s="6">
+        <v>14</v>
+      </c>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6">
+        <v>68</v>
+      </c>
+      <c r="G71" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H71" s="6">
+        <f>(104+158)/2</f>
+        <v>131</v>
+      </c>
+      <c r="I71" s="6">
+        <f>(55+42)/2</f>
+        <v>48.5</v>
+      </c>
+      <c r="J71" s="6">
+        <v>72</v>
+      </c>
+      <c r="K71" s="7"/>
+      <c r="L71" s="24"/>
+      <c r="M71" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B72" s="6"/>
+      <c r="C72" s="6">
+        <v>175</v>
+      </c>
+      <c r="D72" s="6">
+        <v>60</v>
+      </c>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H72" s="6">
+        <v>128</v>
+      </c>
+      <c r="I72" s="6">
+        <v>63</v>
+      </c>
+      <c r="J72" s="6"/>
+      <c r="K72" s="6"/>
+      <c r="L72" s="24"/>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B73" s="6">
+        <v>100</v>
+      </c>
+      <c r="C73" s="6">
+        <v>250</v>
+      </c>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6">
+        <f>(30+60)/2</f>
+        <v>45</v>
+      </c>
+      <c r="G73" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H73" s="6">
+        <v>200</v>
+      </c>
+      <c r="I73" s="6">
+        <v>80</v>
+      </c>
+      <c r="J73" s="6"/>
+      <c r="K73" s="6"/>
+      <c r="L73" s="24"/>
+      <c r="M73" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B74" s="6"/>
+      <c r="C74" s="6">
+        <v>244</v>
+      </c>
+      <c r="D74" s="6">
+        <v>28</v>
+      </c>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H74" s="6">
+        <v>101</v>
+      </c>
+      <c r="I74" s="6"/>
+      <c r="J74" s="6"/>
+      <c r="K74" s="6"/>
+      <c r="L74" s="6"/>
+      <c r="M74" t="s">
         <v>18</v>
       </c>
     </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6">
+        <v>20</v>
+      </c>
+      <c r="F75" s="14">
+        <v>18.8</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H75" s="6"/>
+      <c r="I75" s="6"/>
+      <c r="J75" s="6"/>
+      <c r="K75" s="6"/>
+      <c r="L75" s="6"/>
+      <c r="M75" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B76" s="6"/>
+      <c r="C76" s="6">
+        <v>254</v>
+      </c>
+      <c r="D76" s="6">
+        <f>(41+6)/2</f>
+        <v>23.5</v>
+      </c>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6">
+        <v>104</v>
+      </c>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6">
+        <f>(171+43)/2</f>
+        <v>107</v>
+      </c>
+      <c r="I76" s="6"/>
+      <c r="J76" s="6"/>
+      <c r="K76" s="6"/>
+      <c r="L76" s="6"/>
+      <c r="M76" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B77" s="6"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="6"/>
+      <c r="J77" s="6"/>
+      <c r="K77" s="6"/>
+      <c r="L77" s="6"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B78" s="6"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="6"/>
+      <c r="J78" s="6"/>
+      <c r="K78" s="6"/>
+      <c r="L78" s="6"/>
+    </row>
+    <row r="79" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="8"/>
+      <c r="C79" s="8">
+        <f>AVERAGE(C71:C74)</f>
+        <v>238.5</v>
+      </c>
+      <c r="D79" s="8">
+        <f>AVERAGE(D71:D76)</f>
+        <v>31.375</v>
+      </c>
+      <c r="E79" s="8">
+        <f>AVERAGE(E70:E78)</f>
+        <v>20</v>
+      </c>
+      <c r="F79" s="8">
+        <f>AVERAGE(F71:F75)</f>
+        <v>43.933333333333337</v>
+      </c>
+      <c r="G79" s="8"/>
+      <c r="H79" s="8">
+        <f>AVERAGE(H71:H78)</f>
+        <v>133.4</v>
+      </c>
+      <c r="I79" s="8">
+        <f>AVERAGE(I71:I74)</f>
+        <v>63.833333333333336</v>
+      </c>
+      <c r="J79" s="8">
+        <f>AVERAGE(J70:J78)</f>
+        <v>72</v>
+      </c>
+      <c r="K79" s="8"/>
+      <c r="L79" s="8"/>
+    </row>
+    <row r="80" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B80" s="2"/>
+      <c r="C80" s="3">
+        <f>C79</f>
+        <v>238.5</v>
+      </c>
+      <c r="D80" s="4">
+        <f>D79</f>
+        <v>31.375</v>
+      </c>
+      <c r="E80" s="4">
+        <f>E79</f>
+        <v>20</v>
+      </c>
+      <c r="F80" s="4">
+        <f>F79</f>
+        <v>43.933333333333337</v>
+      </c>
+      <c r="G80" s="4"/>
+      <c r="H80" s="25">
+        <f>AVERAGE(H79:I79)</f>
+        <v>98.616666666666674</v>
+      </c>
+      <c r="I80" s="26"/>
+      <c r="J80" s="4">
+        <f>J79</f>
+        <v>72</v>
+      </c>
+      <c r="K80" s="4">
+        <v>0</v>
+      </c>
+      <c r="L80" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="K81" t="s">
+        <v>15</v>
+      </c>
+      <c r="L81" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="82" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="K82" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="84" spans="2:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="B84" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="85" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I85" s="21"/>
+      <c r="L85" s="21"/>
+    </row>
+    <row r="86" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C86" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D86" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E86" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F86" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G86" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H86" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I86" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="J86" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="K86" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="L86" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M86" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="N86" s="11"/>
+    </row>
+    <row r="87" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>33</v>
+      </c>
+      <c r="C87" t="s">
+        <v>33</v>
+      </c>
+      <c r="D87">
+        <f>D80</f>
+        <v>31.375</v>
+      </c>
+      <c r="E87">
+        <f>(E80+24.9)/2</f>
+        <v>22.45</v>
+      </c>
+      <c r="F87">
+        <f>((F79+100.3)/2)</f>
+        <v>72.116666666666674</v>
+      </c>
+      <c r="G87" t="s">
+        <v>41</v>
+      </c>
+      <c r="H87">
+        <f>(256.2+203.8+254.6)/3</f>
+        <v>238.20000000000002</v>
+      </c>
+      <c r="I87">
+        <f>(201.3+159.5+200)/3</f>
+        <v>186.93333333333331</v>
+      </c>
+      <c r="J87">
+        <f>(122+103.9+134.7)/3</f>
+        <v>120.2</v>
+      </c>
+      <c r="K87" s="4">
+        <v>72</v>
+      </c>
+      <c r="N87" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="88" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L88">
+        <v>10.770460768596649</v>
+      </c>
+      <c r="M88">
+        <v>19.883927572793816</v>
+      </c>
+      <c r="N88" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="89" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L89">
+        <v>53.852303842983247</v>
+      </c>
+      <c r="M89">
+        <v>95.277152952970354</v>
+      </c>
+      <c r="N89" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="90" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L90">
+        <v>124.27454732996134</v>
+      </c>
+      <c r="M90">
+        <v>186.41182099494202</v>
+      </c>
+      <c r="N90" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H80:I80"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="M10" r:id="rId1" xr:uid="{0520E299-4827-774E-99BD-4862E507CCF1}"/>
+    <hyperlink ref="H23" r:id="rId2" xr:uid="{36584DE5-CF96-2E4E-9804-561718E466AD}"/>
+    <hyperlink ref="M75" r:id="rId3" xr:uid="{C7C88F19-537C-1748-9CC5-8413872F53AA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>